<commit_message>
Added diplom on Flask
</commit_message>
<xml_diff>
--- a/Diplom/MonitoringUL/PS_INFO/RZHNK.xlsx
+++ b/Diplom/MonitoringUL/PS_INFO/RZHNK.xlsx
@@ -46,7 +46,7 @@
     <t>Перечень действующих на территории Российской Федерации жилищных накопительных кооперативов, включенных в реестр жилищных накопительных кооперативов по состоянию на dd.mm.yyyy</t>
   </si>
   <si>
-    <t>Перечень действующих на территории Российской Федерации жилищных накопительных кооперативов, включенных в реестр жилищных накопительных кооперативов по состоянию на 17.12.2024</t>
+    <t>Перечень действующих на территории Российской Федерации жилищных накопительных кооперативов, включенных в реестр жилищных накопительных кооперативов по состоянию на 24.12.2024</t>
   </si>
   <si>
     <t>1</t>
@@ -178,7 +178,7 @@
     <t>ЖНК "КБС-ДОМ"</t>
   </si>
   <si>
-    <t>660019, Красноярский край, г. КРАСНОЯРСК, УЛ МУСОРГСКОГО, ЗД. 18, ПОМЕЩ. 110</t>
+    <t>660079, Красноярский край, г. КРАСНОЯРСК, УЛ МУСОРГСКОГО, ЗД. 18, ПОМЕЩ. 110</t>
   </si>
   <si>
     <t>2464062699</t>
@@ -841,7 +841,7 @@
     <t>07.08.2023</t>
   </si>
   <si>
-    <t>367008, Республика Дагестан, г. МАХАЧКАЛА, УЛ ТИТОВА, Д. 144, К. 4, ПОМЕЩ. 12</t>
+    <t>367027, Республика Дагестан, г. МАХАЧКАЛА, УЛ АКУШИНСКОГО 4-Я ЛИНИЯ, Д. 48, ОФИС 10</t>
   </si>
   <si>
     <t>0572034261</t>

</xml_diff>